<commit_message>
Allow for blank cells in XLSX imports
</commit_message>
<xml_diff>
--- a/static/abcd.xlsx
+++ b/static/abcd.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="ABCDsample.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -450,9 +450,6 @@
       </c>
       <c r="B3">
         <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>

</xml_diff>